<commit_message>
Upgraded to Genero 3.20 and ApachePOI 4.1.0
Note: the additional entries in CLASSPATH
</commit_message>
<xml_diff>
--- a/fgl_excel_generic_test.xlsx
+++ b/fgl_excel_generic_test.xlsx
@@ -12,159 +12,171 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
-  <si>
-    <t>23/11/2017</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+  <si>
+    <t>integer_type</t>
+  </si>
+  <si>
+    <t>date_type</t>
+  </si>
+  <si>
+    <t>char_type</t>
+  </si>
+  <si>
+    <t>float_type</t>
+  </si>
+  <si>
+    <t>26/07/2019</t>
   </si>
   <si>
     <t xml:space="preserve">A                   </t>
   </si>
   <si>
-    <t>24/11/2017</t>
+    <t>27/07/2019</t>
   </si>
   <si>
     <t xml:space="preserve">B                   </t>
   </si>
   <si>
-    <t>25/11/2017</t>
+    <t>28/07/2019</t>
   </si>
   <si>
     <t xml:space="preserve">C                   </t>
   </si>
   <si>
-    <t>26/11/2017</t>
+    <t>29/07/2019</t>
   </si>
   <si>
     <t xml:space="preserve">D                   </t>
   </si>
   <si>
-    <t>27/11/2017</t>
+    <t>30/07/2019</t>
   </si>
   <si>
     <t xml:space="preserve">E                   </t>
   </si>
   <si>
-    <t>28/11/2017</t>
+    <t>31/07/2019</t>
   </si>
   <si>
     <t xml:space="preserve">F                   </t>
   </si>
   <si>
-    <t>29/11/2017</t>
+    <t>01/08/2019</t>
   </si>
   <si>
     <t xml:space="preserve">G                   </t>
   </si>
   <si>
-    <t>30/11/2017</t>
+    <t>02/08/2019</t>
   </si>
   <si>
     <t xml:space="preserve">H                   </t>
   </si>
   <si>
-    <t>01/12/2017</t>
+    <t>03/08/2019</t>
   </si>
   <si>
     <t xml:space="preserve">I                   </t>
   </si>
   <si>
-    <t>02/12/2017</t>
+    <t>04/08/2019</t>
   </si>
   <si>
     <t xml:space="preserve">J                   </t>
   </si>
   <si>
-    <t>03/12/2017</t>
+    <t>05/08/2019</t>
   </si>
   <si>
     <t xml:space="preserve">K                   </t>
   </si>
   <si>
-    <t>04/12/2017</t>
+    <t>06/08/2019</t>
   </si>
   <si>
     <t xml:space="preserve">L                   </t>
   </si>
   <si>
-    <t>05/12/2017</t>
+    <t>07/08/2019</t>
   </si>
   <si>
     <t xml:space="preserve">M                   </t>
   </si>
   <si>
-    <t>06/12/2017</t>
+    <t>08/08/2019</t>
   </si>
   <si>
     <t xml:space="preserve">N                   </t>
   </si>
   <si>
-    <t>07/12/2017</t>
+    <t>09/08/2019</t>
   </si>
   <si>
     <t xml:space="preserve">O                   </t>
   </si>
   <si>
-    <t>08/12/2017</t>
+    <t>10/08/2019</t>
   </si>
   <si>
     <t xml:space="preserve">P                   </t>
   </si>
   <si>
-    <t>09/12/2017</t>
+    <t>11/08/2019</t>
   </si>
   <si>
     <t xml:space="preserve">Q                   </t>
   </si>
   <si>
-    <t>10/12/2017</t>
+    <t>12/08/2019</t>
   </si>
   <si>
     <t xml:space="preserve">R                   </t>
   </si>
   <si>
-    <t>11/12/2017</t>
+    <t>13/08/2019</t>
   </si>
   <si>
     <t xml:space="preserve">S                   </t>
   </si>
   <si>
-    <t>12/12/2017</t>
+    <t>14/08/2019</t>
   </si>
   <si>
     <t xml:space="preserve">T                   </t>
   </si>
   <si>
-    <t>13/12/2017</t>
+    <t>15/08/2019</t>
   </si>
   <si>
     <t xml:space="preserve">U                   </t>
   </si>
   <si>
-    <t>14/12/2017</t>
+    <t>16/08/2019</t>
   </si>
   <si>
     <t xml:space="preserve">V                   </t>
   </si>
   <si>
-    <t>15/12/2017</t>
+    <t>17/08/2019</t>
   </si>
   <si>
     <t xml:space="preserve">W                   </t>
   </si>
   <si>
-    <t>16/12/2017</t>
+    <t>18/08/2019</t>
   </si>
   <si>
     <t xml:space="preserve">X                   </t>
   </si>
   <si>
-    <t>17/12/2017</t>
+    <t>19/08/2019</t>
   </si>
   <si>
     <t xml:space="preserve">Y                   </t>
   </si>
   <si>
-    <t>18/12/2017</t>
+    <t>20/08/2019</t>
   </si>
   <si>
     <t xml:space="preserve">Z                   </t>
@@ -175,13 +187,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -204,381 +221,398 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="D1" t="n">
-        <v>1.0</v>
+      <c r="C1" t="s" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D3" t="n">
-        <v>0.333333333333333</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" t="n">
-        <v>0.25</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D6" t="n">
-        <v>0.166666666666667</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D7" t="n">
-        <v>0.142857142857143</v>
+        <v>0.166666666666667</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D8" t="n">
-        <v>0.125</v>
+        <v>0.142857142857143</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D9" t="n">
-        <v>0.111111111111111</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1</v>
+        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0909090909090909</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0833333333333333</v>
+        <v>0.0909090909090909</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0769230769230769</v>
+        <v>0.0833333333333333</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0714285714285714</v>
+        <v>0.0769230769230769</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0666666666666667</v>
+        <v>0.0714285714285714</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>16.0</v>
+        <v>15.0</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0625</v>
+        <v>0.0666666666666667</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>17.0</v>
+        <v>16.0</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0588235294117647</v>
+        <v>0.0625</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>18.0</v>
+        <v>17.0</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0555555555555556</v>
+        <v>0.0588235294117647</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>19.0</v>
+        <v>18.0</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0526315789473684</v>
+        <v>0.0555555555555556</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>20.0</v>
+        <v>19.0</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D20" t="n">
-        <v>0.05</v>
+        <v>0.0526315789473684</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>21.0</v>
+        <v>20.0</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0476190476190476</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>22.0</v>
+        <v>21.0</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0454545454545455</v>
+        <v>0.0476190476190476</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>23.0</v>
+        <v>22.0</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0434782608695652</v>
+        <v>0.0454545454545455</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>24.0</v>
+        <v>23.0</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0416666666666667</v>
+        <v>0.0434782608695652</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>25.0</v>
+        <v>24.0</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D25" t="n">
-        <v>0.04</v>
+        <v>0.0416666666666667</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
         <v>26.0</v>
       </c>
-      <c r="B26" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" t="n">
+      <c r="B27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" t="n">
         <v>0.0384615384615385</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed post WWDC19, including  in Excel adding code that show number and string values of typical code e.g. 00100.  Changed setcolumnwidth to do the *256 for you
</commit_message>
<xml_diff>
--- a/fgl_excel_generic_test.xlsx
+++ b/fgl_excel_generic_test.xlsx
@@ -26,157 +26,157 @@
     <t>float_type</t>
   </si>
   <si>
-    <t>26/07/2019</t>
+    <t>04/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">A                   </t>
   </si>
   <si>
-    <t>27/07/2019</t>
+    <t>05/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">B                   </t>
   </si>
   <si>
-    <t>28/07/2019</t>
+    <t>06/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">C                   </t>
   </si>
   <si>
-    <t>29/07/2019</t>
+    <t>07/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">D                   </t>
   </si>
   <si>
-    <t>30/07/2019</t>
+    <t>08/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">E                   </t>
   </si>
   <si>
-    <t>31/07/2019</t>
+    <t>09/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">F                   </t>
   </si>
   <si>
-    <t>01/08/2019</t>
+    <t>10/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">G                   </t>
   </si>
   <si>
-    <t>02/08/2019</t>
+    <t>11/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">H                   </t>
   </si>
   <si>
-    <t>03/08/2019</t>
+    <t>12/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">I                   </t>
   </si>
   <si>
-    <t>04/08/2019</t>
+    <t>13/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">J                   </t>
   </si>
   <si>
-    <t>05/08/2019</t>
+    <t>14/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">K                   </t>
   </si>
   <si>
-    <t>06/08/2019</t>
+    <t>15/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">L                   </t>
   </si>
   <si>
-    <t>07/08/2019</t>
+    <t>16/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">M                   </t>
   </si>
   <si>
-    <t>08/08/2019</t>
+    <t>17/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">N                   </t>
   </si>
   <si>
-    <t>09/08/2019</t>
+    <t>18/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">O                   </t>
   </si>
   <si>
-    <t>10/08/2019</t>
+    <t>19/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">P                   </t>
   </si>
   <si>
-    <t>11/08/2019</t>
+    <t>20/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">Q                   </t>
   </si>
   <si>
-    <t>12/08/2019</t>
+    <t>21/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">R                   </t>
   </si>
   <si>
-    <t>13/08/2019</t>
+    <t>22/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">S                   </t>
   </si>
   <si>
-    <t>14/08/2019</t>
+    <t>23/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">T                   </t>
   </si>
   <si>
-    <t>15/08/2019</t>
+    <t>24/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">U                   </t>
   </si>
   <si>
-    <t>16/08/2019</t>
+    <t>25/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">V                   </t>
   </si>
   <si>
-    <t>17/08/2019</t>
+    <t>26/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">W                   </t>
   </si>
   <si>
-    <t>18/08/2019</t>
+    <t>27/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">X                   </t>
   </si>
   <si>
-    <t>19/08/2019</t>
+    <t>28/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">Y                   </t>
   </si>
   <si>
-    <t>20/08/2019</t>
+    <t>29/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">Z                   </t>

</xml_diff>

<commit_message>
Added  ability to import and read Word document Added ability to open a Word template as a starting point
</commit_message>
<xml_diff>
--- a/fgl_excel_generic_test.xlsx
+++ b/fgl_excel_generic_test.xlsx
@@ -26,157 +26,157 @@
     <t>float_type</t>
   </si>
   <si>
-    <t>04/10/2019</t>
+    <t>05/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">A                   </t>
   </si>
   <si>
-    <t>05/10/2019</t>
+    <t>06/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">B                   </t>
   </si>
   <si>
-    <t>06/10/2019</t>
+    <t>07/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">C                   </t>
   </si>
   <si>
-    <t>07/10/2019</t>
+    <t>08/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">D                   </t>
   </si>
   <si>
-    <t>08/10/2019</t>
+    <t>09/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">E                   </t>
   </si>
   <si>
-    <t>09/10/2019</t>
+    <t>10/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">F                   </t>
   </si>
   <si>
-    <t>10/10/2019</t>
+    <t>11/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">G                   </t>
   </si>
   <si>
-    <t>11/10/2019</t>
+    <t>12/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">H                   </t>
   </si>
   <si>
-    <t>12/10/2019</t>
+    <t>13/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">I                   </t>
   </si>
   <si>
-    <t>13/10/2019</t>
+    <t>14/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">J                   </t>
   </si>
   <si>
-    <t>14/10/2019</t>
+    <t>15/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">K                   </t>
   </si>
   <si>
-    <t>15/10/2019</t>
+    <t>16/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">L                   </t>
   </si>
   <si>
-    <t>16/10/2019</t>
+    <t>17/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">M                   </t>
   </si>
   <si>
-    <t>17/10/2019</t>
+    <t>18/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">N                   </t>
   </si>
   <si>
-    <t>18/10/2019</t>
+    <t>19/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">O                   </t>
   </si>
   <si>
-    <t>19/10/2019</t>
+    <t>20/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">P                   </t>
   </si>
   <si>
-    <t>20/10/2019</t>
+    <t>21/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">Q                   </t>
   </si>
   <si>
-    <t>21/10/2019</t>
+    <t>22/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">R                   </t>
   </si>
   <si>
-    <t>22/10/2019</t>
+    <t>23/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">S                   </t>
   </si>
   <si>
-    <t>23/10/2019</t>
+    <t>24/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">T                   </t>
   </si>
   <si>
-    <t>24/10/2019</t>
+    <t>25/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">U                   </t>
   </si>
   <si>
-    <t>25/10/2019</t>
+    <t>26/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">V                   </t>
   </si>
   <si>
-    <t>26/10/2019</t>
+    <t>27/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">W                   </t>
   </si>
   <si>
-    <t>27/10/2019</t>
+    <t>28/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">X                   </t>
   </si>
   <si>
-    <t>28/10/2019</t>
+    <t>29/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">Y                   </t>
   </si>
   <si>
-    <t>29/10/2019</t>
+    <t>30/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">Z                   </t>
@@ -223,7 +223,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="true" applyFont="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>

</xml_diff>